<commit_message>
added exp 2 xcel
</commit_message>
<xml_diff>
--- a/PlantTransTwo/PlantTransII_Exp1.xlsx
+++ b/PlantTransTwo/PlantTransII_Exp1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipburnham/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipburnham/Documents/GitHub/Dissertation/PlantTransTwo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -177,10 +177,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$60</c:f>
+              <c:f>Sheet1!$D$2:$D$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>17.0</c:v>
                 </c:pt>
@@ -351,22 +351,16 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$60</c:f>
+              <c:f>Sheet1!$E$2:$E$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -536,12 +530,6 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
                   <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -557,11 +545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="615294512"/>
-        <c:axId val="588007968"/>
+        <c:axId val="-1298980656"/>
+        <c:axId val="-1298976464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="615294512"/>
+        <c:axId val="-1298980656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,12 +605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588007968"/>
+        <c:crossAx val="-1298976464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="588007968"/>
+        <c:axId val="-1298976464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="615294512"/>
+        <c:crossAx val="-1298980656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1581,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2575,40 +2563,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>61</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>4</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>